<commit_message>
correct height, weight, waist methods, diabetes type
</commit_message>
<xml_diff>
--- a/longitudinal/data_processing_elements_longitudinal-MSN.xlsx
+++ b/longitudinal/data_processing_elements_longitudinal-MSN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F30FED-DDA2-4BB5-B1AC-C24A1CFC130F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369A09A5-EDAE-4543-A741-F332390DBDE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DE4C7F53-17AD-41A0-BCA9-A2A8E85C7880}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DE4C7F53-17AD-41A0-BCA9-A2A8E85C7880}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="401">
   <si>
     <t>index</t>
   </si>
@@ -1113,9 +1113,6 @@
 1 = history of CVD ; 
 0 = no history of CVD ; 
 1 = history of CVD</t>
-  </si>
-  <si>
-    <t>N_GTS_WHO ; N_GTS_WHO.ph2</t>
   </si>
   <si>
     <t>glucose tolerance status according to WHO ; glucose tolerance status according to WHO</t>
@@ -1628,22 +1625,10 @@
     <t>Height (cm)</t>
   </si>
   <si>
-    <t>case_when(!is.na(Height.ph2),2,NA)</t>
-  </si>
-  <si>
     <t>Weight.ph2</t>
   </si>
   <si>
     <t>bmi.ph2</t>
-  </si>
-  <si>
-    <t>waistph2</t>
-  </si>
-  <si>
-    <t>case_when(!is.na(Weight.ph2),2,NA)</t>
-  </si>
-  <si>
-    <t>case_when(!is.na(waistph2),2,NA)</t>
   </si>
   <si>
     <t>OSBP.ph2</t>
@@ -1739,6 +1724,21 @@
   </si>
   <si>
     <t>recode(1=4;2=4;3=3;4=2;5=1)</t>
+  </si>
+  <si>
+    <t>case_when(!is.na(Height.ph2)~2;
+ELSE~NA)</t>
+  </si>
+  <si>
+    <t>case_when(!is.na(Weight.ph2)~2;
+ELSE~NA)</t>
+  </si>
+  <si>
+    <t>waist.ph2</t>
+  </si>
+  <si>
+    <t>case_when(!is.na(waist.ph2)~2;
+ELSE~NA)</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1894,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2212,11 +2212,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A617E81B-AA39-4B57-8286-9F6F09A3BC0B}">
   <dimension ref="A1:AD166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="M13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
@@ -2404,7 +2404,7 @@
         <v>36</v>
       </c>
       <c r="V3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="W3" s="7">
         <v>2</v>
@@ -2434,10 +2434,10 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P4" t="s">
         <v>45</v>
@@ -2453,7 +2453,7 @@
         <v>47</v>
       </c>
       <c r="W4" s="14" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>299</v>
@@ -2549,7 +2549,7 @@
         <v>279</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="165" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
         <v>285</v>
       </c>
       <c r="J8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>302</v>
@@ -2630,10 +2630,10 @@
         <v>34</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="T8" t="s">
         <v>35</v>
@@ -2645,7 +2645,7 @@
         <v>52</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="60" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>286</v>
       </c>
       <c r="J12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>304</v>
@@ -2792,7 +2792,7 @@
         <v>34</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T12" t="s">
         <v>35</v>
@@ -2804,7 +2804,7 @@
         <v>52</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2830,7 +2830,7 @@
         <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>303</v>
@@ -2839,13 +2839,13 @@
         <v>34</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T13" t="s">
         <v>62</v>
       </c>
       <c r="U13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="V13" t="s">
         <v>62</v>
@@ -2880,7 +2880,7 @@
         <v>282</v>
       </c>
       <c r="J14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>303</v>
@@ -2889,7 +2889,7 @@
         <v>34</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="T14" t="s">
         <v>35</v>
@@ -2901,7 +2901,7 @@
         <v>52</v>
       </c>
       <c r="W14" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
@@ -2967,10 +2967,10 @@
       </c>
       <c r="I16" s="1"/>
       <c r="J16" t="s">
+        <v>364</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="M16"/>
       <c r="P16" t="s">
@@ -3015,10 +3015,10 @@
         <v>96</v>
       </c>
       <c r="J17" t="s">
+        <v>364</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="M17"/>
       <c r="T17" t="s">
@@ -3030,8 +3030,8 @@
       <c r="V17" t="s">
         <v>279</v>
       </c>
-      <c r="W17" t="s">
-        <v>367</v>
+      <c r="W17" s="1" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="I18" s="1"/>
       <c r="J18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>307</v>
@@ -3083,7 +3083,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>96</v>
       </c>
       <c r="J19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="M19"/>
       <c r="T19" t="s">
@@ -3118,8 +3118,8 @@
       <c r="V19" t="s">
         <v>279</v>
       </c>
-      <c r="W19" t="s">
-        <v>371</v>
+      <c r="W19" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="45" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
         <v>104</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>308</v>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>370</v>
+        <v>399</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>311</v>
@@ -3241,8 +3241,8 @@
       <c r="I22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J22" t="s">
-        <v>370</v>
+      <c r="J22" s="1" t="s">
+        <v>399</v>
       </c>
       <c r="M22"/>
       <c r="T22" t="s">
@@ -3254,8 +3254,8 @@
       <c r="V22" t="s">
         <v>279</v>
       </c>
-      <c r="W22" t="s">
-        <v>372</v>
+      <c r="W22" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -3365,7 +3365,7 @@
         <v>117</v>
       </c>
       <c r="J25" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>309</v>
@@ -3413,7 +3413,7 @@
         <v>117</v>
       </c>
       <c r="J26" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>310</v>
@@ -3461,7 +3461,7 @@
         <v>123</v>
       </c>
       <c r="J27" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>315</v>
@@ -3471,7 +3471,7 @@
         <v>73</v>
       </c>
       <c r="R27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="T27" t="s">
         <v>35</v>
@@ -3630,7 +3630,7 @@
         <v>134</v>
       </c>
       <c r="J31" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>316</v>
@@ -3678,7 +3678,7 @@
         <v>137</v>
       </c>
       <c r="J32" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>317</v>
@@ -3726,7 +3726,7 @@
         <v>137</v>
       </c>
       <c r="J33" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>319</v>
@@ -3751,7 +3751,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>137</v>
       </c>
       <c r="J34" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>320</v>
@@ -3822,10 +3822,10 @@
         <v>137</v>
       </c>
       <c r="J35" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M35"/>
       <c r="P35" t="s">
@@ -3844,7 +3844,7 @@
         <v>47</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="X35" t="s">
         <v>321</v>
@@ -3873,7 +3873,7 @@
         <v>137</v>
       </c>
       <c r="J36" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>318</v>
@@ -4149,7 +4149,7 @@
         <v>165</v>
       </c>
       <c r="J42" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>326</v>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="I43" s="1"/>
       <c r="J43" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>327</v>
@@ -4291,7 +4291,7 @@
         <v>288</v>
       </c>
       <c r="J45" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>328</v>
@@ -4301,7 +4301,7 @@
         <v>34</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="T45" t="s">
         <v>35</v>
@@ -4313,7 +4313,7 @@
         <v>52</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4418,7 +4418,7 @@
         <v>290</v>
       </c>
       <c r="J48" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>329</v>
@@ -4428,7 +4428,7 @@
         <v>34</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="T48" t="s">
         <v>35</v>
@@ -4440,7 +4440,7 @@
         <v>52</v>
       </c>
       <c r="W48" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="135" x14ac:dyDescent="0.25">
@@ -4466,7 +4466,7 @@
         <v>185</v>
       </c>
       <c r="J49" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>330</v>
@@ -4553,17 +4553,17 @@
         <v>185</v>
       </c>
       <c r="J51" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M51"/>
       <c r="P51" t="s">
         <v>34</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="T51" t="s">
         <v>35</v>
@@ -4575,7 +4575,7 @@
         <v>52</v>
       </c>
       <c r="W51" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="52" spans="1:24" ht="165" x14ac:dyDescent="0.25">
@@ -4601,17 +4601,17 @@
         <v>291</v>
       </c>
       <c r="J52" t="s">
+        <v>383</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="M52"/>
       <c r="P52" t="s">
         <v>34</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="T52" t="s">
         <v>35</v>
@@ -4623,7 +4623,7 @@
         <v>52</v>
       </c>
       <c r="W52" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="1:24" ht="30" x14ac:dyDescent="0.25">
@@ -4727,17 +4727,17 @@
         <v>185</v>
       </c>
       <c r="J55" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M55"/>
       <c r="P55" t="s">
         <v>34</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T55" t="s">
         <v>35</v>
@@ -4752,7 +4752,7 @@
         <v>93</v>
       </c>
       <c r="X55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="56" spans="1:24" ht="75" x14ac:dyDescent="0.25">
@@ -4778,17 +4778,17 @@
         <v>185</v>
       </c>
       <c r="J56" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M56"/>
       <c r="P56" t="s">
         <v>34</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T56" t="s">
         <v>35</v>
@@ -5025,7 +5025,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:24" ht="390" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="360" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>64</v>
       </c>
@@ -5045,10 +5045,10 @@
         <v>40</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O63" s="1"/>
       <c r="P63" t="s">
@@ -5064,7 +5064,7 @@
         <v>47</v>
       </c>
       <c r="W63" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
@@ -5140,7 +5140,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="105" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>67</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>68</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>71</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="90" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>72</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>75</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>76</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:24" ht="135" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="165" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>78</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="75" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>79</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="90" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="120" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>80</v>
       </c>
@@ -5789,17 +5789,17 @@
         <v>185</v>
       </c>
       <c r="J82" s="9" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="M82"/>
       <c r="P82" t="s">
         <v>73</v>
       </c>
       <c r="R82" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="T82" t="s">
         <v>35</v>
@@ -5811,10 +5811,10 @@
         <v>279</v>
       </c>
       <c r="W82" s="1" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="X82" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="83" spans="1:24" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
@@ -5837,10 +5837,10 @@
         <v>73</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="M83"/>
       <c r="P83" t="s">
@@ -5856,7 +5856,7 @@
         <v>47</v>
       </c>
       <c r="W83" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="84" spans="1:24" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
@@ -5882,16 +5882,16 @@
         <v>278</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P84" t="s">
         <v>34</v>
       </c>
       <c r="Q84" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="T84" t="s">
         <v>35</v>
@@ -5903,7 +5903,7 @@
         <v>47</v>
       </c>
       <c r="W84" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>